<commit_message>
commit for project completion!
</commit_message>
<xml_diff>
--- a/Manual testing/Project/Scenario.xlsx
+++ b/Manual testing/Project/Scenario.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>Test Scenatio ID</t>
   </si>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>P3</t>
-  </si>
-  <si>
-    <t>https://demoqa.com/interaction</t>
   </si>
 </sst>
 </file>
@@ -462,10 +459,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -750,40 +747,48 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A17" s="3"/>
+      <c r="A17" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="B17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E18" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>48</v>
@@ -794,35 +799,18 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E20" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="3">
         <v>5</v>
       </c>
     </row>
@@ -836,8 +824,8 @@
     <hyperlink ref="B11:B12" r:id="rId6" display="https://demoqa.com/alertsWindows"/>
     <hyperlink ref="B13" r:id="rId7"/>
     <hyperlink ref="B14:B16" r:id="rId8" display="https://demoqa.com/widgets"/>
-    <hyperlink ref="B18" r:id="rId9"/>
-    <hyperlink ref="B19:B21" r:id="rId10" display="https://demoqa.com/bookstore"/>
+    <hyperlink ref="B17" r:id="rId9"/>
+    <hyperlink ref="B18:B20" r:id="rId10" display="https://demoqa.com/bookstore"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>

</xml_diff>